<commit_message>
Added Sprint Review Power Point
</commit_message>
<xml_diff>
--- a/Documents/BackLog.xlsx
+++ b/Documents/BackLog.xlsx
@@ -8,6 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -132,8 +133,34 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -152,11 +179,37 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="31">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -489,7 +542,7 @@
   <dimension ref="A1:J43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection sqref="A1:C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -550,11 +603,11 @@
       <c r="A4" s="3">
         <v>3</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>5</v>
+      <c r="B4" s="3" t="s">
+        <v>12</v>
       </c>
       <c r="C4" s="3">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
@@ -569,10 +622,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C5" s="3">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
@@ -586,11 +639,11 @@
       <c r="A6" s="3">
         <v>5</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>6</v>
+      <c r="B6" s="1" t="s">
+        <v>5</v>
       </c>
       <c r="C6" s="3">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
@@ -605,10 +658,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C7" s="3">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
@@ -623,10 +676,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="C8" s="3">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
@@ -1119,4 +1172,21 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Some additions to sprinklers and test case document added
</commit_message>
<xml_diff>
--- a/Documents/BackLog.xlsx
+++ b/Documents/BackLog.xlsx
@@ -836,8 +836,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="E70" sqref="E70"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="C63" sqref="C63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
Added Sprint Review 2 power point
</commit_message>
<xml_diff>
--- a/Documents/BackLog.xlsx
+++ b/Documents/BackLog.xlsx
@@ -4,11 +4,10 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-440" windowWidth="28800" windowHeight="18000" tabRatio="500"/>
+    <workbookView xWindow="720" yWindow="740" windowWidth="25540" windowHeight="15980" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="80">
   <si>
     <t>Priority</t>
   </si>
@@ -267,6 +266,39 @@
   </si>
   <si>
     <t xml:space="preserve">Code Fire Sensors </t>
+  </si>
+  <si>
+    <t>Sprint 1 Left Over</t>
+  </si>
+  <si>
+    <t>Sprint 2 Left Over</t>
+  </si>
+  <si>
+    <t>US-02.1</t>
+  </si>
+  <si>
+    <t>Done Points</t>
+  </si>
+  <si>
+    <t>US-03.1</t>
+  </si>
+  <si>
+    <t>Alarm On/Off at specific Times(Added After Sprint 1)</t>
+  </si>
+  <si>
+    <t>Log Out of web interface (Added After Sprint 1)</t>
+  </si>
+  <si>
+    <t>US-04.1</t>
+  </si>
+  <si>
+    <t>Turn Alarm on/off</t>
+  </si>
+  <si>
+    <t>Code Contact Fire Deparment</t>
+  </si>
+  <si>
+    <t>Code Contact Homeowners</t>
   </si>
 </sst>
 </file>
@@ -336,7 +368,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -346,6 +378,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -373,7 +411,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="46">
+  <cellStyleXfs count="106">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -420,8 +458,68 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -458,8 +556,15 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="31" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="31" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="31" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="31" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="46">
+  <cellStyles count="106">
     <cellStyle name="Check Cell" xfId="31" builtinId="23"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -483,6 +588,36 @@
     <cellStyle name="Followed Hyperlink" xfId="41" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="43" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="45" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="47" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="49" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="51" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="53" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="55" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="57" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="59" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="61" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="63" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="65" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="67" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="69" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="71" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="73" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="75" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="77" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="79" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="81" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="83" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="85" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="87" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="89" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="91" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="93" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="95" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="97" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="99" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="101" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="103" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="105" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -505,6 +640,36 @@
     <cellStyle name="Hyperlink" xfId="40" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="42" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="44" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="46" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="48" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="50" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="52" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="54" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="56" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="58" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="60" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="62" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="64" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="66" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="68" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="70" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="72" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="74" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="76" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="78" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="80" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="82" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="84" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="86" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="88" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="90" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="92" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="94" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="96" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="98" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="100" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="102" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="104" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -834,10 +999,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K65"/>
+  <dimension ref="A1:K71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="C63" sqref="C63"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -847,6 +1012,7 @@
     <col min="4" max="4" width="25.1640625" customWidth="1"/>
     <col min="5" max="5" width="24.5" customWidth="1"/>
     <col min="6" max="6" width="32.33203125" customWidth="1"/>
+    <col min="7" max="7" width="13.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -862,6 +1028,12 @@
       <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
+      <c r="E1" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="4">
@@ -877,8 +1049,12 @@
       <c r="D2" s="4">
         <v>10</v>
       </c>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
+      <c r="E2" s="2">
+        <v>10</v>
+      </c>
+      <c r="F2" s="2">
+        <v>5</v>
+      </c>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
@@ -887,7 +1063,7 @@
     </row>
     <row r="3" spans="1:11" ht="37" customHeight="1">
       <c r="A3" s="4">
-        <f t="shared" ref="A3:A17" si="0">ROW()-1</f>
+        <f t="shared" ref="A3:A19" si="0">ROW()-1</f>
         <v>2</v>
       </c>
       <c r="B3" s="6" t="s">
@@ -899,30 +1075,33 @@
       <c r="D3" s="4">
         <v>5</v>
       </c>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
+      <c r="E3" s="2">
+        <v>0</v>
+      </c>
+      <c r="F3" s="2">
+        <v>0</v>
+      </c>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
     </row>
-    <row r="4" spans="1:11" ht="30">
-      <c r="A4" s="4">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
+    <row r="4" spans="1:11" ht="37" customHeight="1">
+      <c r="A4" s="4"/>
       <c r="B4" s="6" t="s">
-        <v>22</v>
+        <v>71</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>8</v>
+        <v>75</v>
       </c>
       <c r="D4" s="4">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
+      <c r="F4" s="2">
+        <v>0</v>
+      </c>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
@@ -935,38 +1114,41 @@
         <v>4</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D5" s="4">
         <v>10</v>
       </c>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
+      <c r="E5" s="2">
+        <v>3</v>
+      </c>
+      <c r="F5" s="2">
+        <v>0</v>
+      </c>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
     </row>
-    <row r="6" spans="1:11" ht="30">
-      <c r="A6" s="4">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
+    <row r="6" spans="1:11">
+      <c r="A6" s="4"/>
       <c r="B6" s="6" t="s">
-        <v>20</v>
+        <v>73</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>13</v>
+        <v>74</v>
       </c>
       <c r="D6" s="4">
         <v>2</v>
       </c>
       <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
+      <c r="F6" s="2">
+        <v>0</v>
+      </c>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
@@ -979,16 +1161,20 @@
         <v>6</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D7" s="4">
-        <v>5</v>
-      </c>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
+        <v>10</v>
+      </c>
+      <c r="E7" s="2">
+        <v>4</v>
+      </c>
+      <c r="F7" s="2">
+        <v>2</v>
+      </c>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
@@ -1001,38 +1187,44 @@
         <v>7</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="D8" s="4">
-        <v>5</v>
-      </c>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
+        <v>2</v>
+      </c>
+      <c r="E8" s="2">
+        <v>1</v>
+      </c>
+      <c r="F8" s="2">
+        <v>1</v>
+      </c>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" ht="30">
       <c r="A9" s="4">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D9" s="4">
         <v>5</v>
       </c>
       <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
+      <c r="F9" s="2">
+        <v>4</v>
+      </c>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
@@ -1045,16 +1237,18 @@
         <v>9</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D10" s="4">
         <v>5</v>
       </c>
       <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
+      <c r="F10" s="2">
+        <v>4</v>
+      </c>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
@@ -1067,35 +1261,37 @@
         <v>10</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D11" s="4">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
+      <c r="F11" s="2">
+        <v>5</v>
+      </c>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
     </row>
-    <row r="12" spans="1:11" ht="30">
+    <row r="12" spans="1:11">
       <c r="A12" s="4">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D12" s="4">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
@@ -1111,13 +1307,13 @@
         <v>12</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="D13" s="4">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
@@ -1127,16 +1323,16 @@
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:11" ht="30">
       <c r="A14" s="4">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D14" s="4">
         <v>10</v>
@@ -1155,13 +1351,13 @@
         <v>14</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="D15" s="4">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
@@ -1171,19 +1367,19 @@
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
     </row>
-    <row r="16" spans="1:11" ht="30">
+    <row r="16" spans="1:11">
       <c r="A16" s="4">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="D16" s="4">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
@@ -1199,13 +1395,13 @@
         <v>16</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D17" s="4">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
@@ -1215,11 +1411,20 @@
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
     </row>
-    <row r="18" spans="1:11">
-      <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
+    <row r="18" spans="1:11" ht="30">
+      <c r="A18" s="4">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" s="4">
+        <v>5</v>
+      </c>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
@@ -1228,11 +1433,20 @@
       <c r="J18" s="2"/>
       <c r="K18" s="2"/>
     </row>
-    <row r="19" spans="1:11">
-      <c r="A19" s="2"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
+    <row r="19" spans="1:11" ht="30">
+      <c r="A19" s="4">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19" s="4">
+        <v>5</v>
+      </c>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
@@ -1242,9 +1456,7 @@
       <c r="K19" s="2"/>
     </row>
     <row r="20" spans="1:11">
-      <c r="A20" s="7" t="s">
-        <v>38</v>
-      </c>
+      <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
@@ -1256,95 +1468,97 @@
       <c r="J20" s="2"/>
       <c r="K20" s="2"/>
     </row>
-    <row r="21" spans="1:11" ht="16" thickBot="1">
-      <c r="A21" s="7"/>
-      <c r="B21" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C21" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="D21" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="E21" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="F21" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="G21" s="7"/>
-      <c r="H21" s="7"/>
+    <row r="21" spans="1:11">
+      <c r="A21" s="2"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
       <c r="K21" s="2"/>
     </row>
-    <row r="22" spans="1:11" ht="17" thickTop="1" thickBot="1">
-      <c r="A22" s="2"/>
-      <c r="B22" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="C22" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="D22" s="10"/>
-      <c r="E22" s="10"/>
-      <c r="F22" s="10"/>
+    <row r="22" spans="1:11">
+      <c r="A22" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
       <c r="K22" s="2"/>
     </row>
-    <row r="23" spans="1:11" ht="16" thickTop="1">
-      <c r="A23" s="2"/>
-      <c r="B23" s="2"/>
-      <c r="C23" s="1"/>
-      <c r="D23" t="s">
-        <v>45</v>
-      </c>
-      <c r="G23" s="2"/>
-      <c r="H23" s="2"/>
+    <row r="23" spans="1:11" ht="16" thickBot="1">
+      <c r="A23" s="7"/>
+      <c r="B23" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="F23" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="G23" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="H23" s="7"/>
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
       <c r="K23" s="2"/>
     </row>
-    <row r="24" spans="1:11" ht="16" thickBot="1">
+    <row r="24" spans="1:11" ht="17" thickTop="1" thickBot="1">
       <c r="A24" s="2"/>
-      <c r="B24" s="2"/>
-      <c r="C24" s="1"/>
-      <c r="D24" t="s">
-        <v>44</v>
-      </c>
-      <c r="G24" s="2"/>
+      <c r="B24" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D24" s="10"/>
+      <c r="E24" s="10"/>
+      <c r="F24" s="10"/>
+      <c r="G24" s="2">
+        <v>0</v>
+      </c>
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
       <c r="K24" s="2"/>
     </row>
-    <row r="25" spans="1:11" ht="32" thickTop="1" thickBot="1">
+    <row r="25" spans="1:11" ht="16" thickTop="1">
       <c r="A25" s="2"/>
-      <c r="B25" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="C25" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="D25" s="10"/>
-      <c r="E25" s="10"/>
-      <c r="F25" s="10"/>
+      <c r="B25" s="2"/>
+      <c r="C25" s="1"/>
+      <c r="D25" t="s">
+        <v>45</v>
+      </c>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
       <c r="K25" s="2"/>
     </row>
-    <row r="26" spans="1:11" ht="17" thickTop="1" thickBot="1">
+    <row r="26" spans="1:11" ht="16" thickBot="1">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="1"/>
-      <c r="F26" t="s">
-        <v>46</v>
+      <c r="D26" t="s">
+        <v>44</v>
       </c>
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
@@ -1355,26 +1569,28 @@
     <row r="27" spans="1:11" ht="32" thickTop="1" thickBot="1">
       <c r="A27" s="2"/>
       <c r="B27" s="8" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D27" s="10"/>
       <c r="E27" s="10"/>
       <c r="F27" s="10"/>
-      <c r="G27" s="2"/>
+      <c r="G27" s="2">
+        <v>5</v>
+      </c>
       <c r="H27" s="2"/>
       <c r="I27" s="2"/>
       <c r="J27" s="2"/>
       <c r="K27" s="2"/>
     </row>
-    <row r="28" spans="1:11" ht="16" thickTop="1">
+    <row r="28" spans="1:11" ht="17" thickTop="1" thickBot="1">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="1"/>
-      <c r="E28" s="11" t="s">
-        <v>49</v>
+      <c r="F28" t="s">
+        <v>46</v>
       </c>
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
@@ -1382,25 +1598,31 @@
       <c r="J28" s="2"/>
       <c r="K28" s="2"/>
     </row>
-    <row r="29" spans="1:11">
+    <row r="29" spans="1:11" ht="32" thickTop="1" thickBot="1">
       <c r="A29" s="2"/>
-      <c r="B29" s="2"/>
-      <c r="C29" s="1"/>
-      <c r="E29" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="G29" s="2"/>
+      <c r="B29" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D29" s="10"/>
+      <c r="E29" s="10"/>
+      <c r="F29" s="10"/>
+      <c r="G29" s="2">
+        <v>7</v>
+      </c>
       <c r="H29" s="2"/>
       <c r="I29" s="2"/>
       <c r="J29" s="2"/>
       <c r="K29" s="2"/>
     </row>
-    <row r="30" spans="1:11">
+    <row r="30" spans="1:11" ht="16" thickTop="1">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="1"/>
-      <c r="F30" t="s">
-        <v>48</v>
+      <c r="E30" s="11" t="s">
+        <v>49</v>
       </c>
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
@@ -1408,12 +1630,12 @@
       <c r="J30" s="2"/>
       <c r="K30" s="2"/>
     </row>
-    <row r="31" spans="1:11" ht="16" thickBot="1">
+    <row r="31" spans="1:11">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="1"/>
-      <c r="F31" t="s">
-        <v>40</v>
+      <c r="E31" s="11" t="s">
+        <v>47</v>
       </c>
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
@@ -1421,29 +1643,25 @@
       <c r="J31" s="2"/>
       <c r="K31" s="2"/>
     </row>
-    <row r="32" spans="1:11" ht="32" thickTop="1" thickBot="1">
+    <row r="32" spans="1:11">
       <c r="A32" s="2"/>
-      <c r="B32" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="C32" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D32" s="10"/>
-      <c r="E32" s="10"/>
-      <c r="F32" s="10"/>
+      <c r="B32" s="2"/>
+      <c r="C32" s="1"/>
+      <c r="F32" t="s">
+        <v>48</v>
+      </c>
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
       <c r="I32" s="2"/>
       <c r="J32" s="2"/>
       <c r="K32" s="2"/>
     </row>
-    <row r="33" spans="1:11" ht="16" thickTop="1">
+    <row r="33" spans="1:11" ht="16" thickBot="1">
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
       <c r="C33" s="1"/>
-      <c r="D33" t="s">
-        <v>52</v>
+      <c r="F33" t="s">
+        <v>40</v>
       </c>
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
@@ -1451,25 +1669,31 @@
       <c r="J33" s="2"/>
       <c r="K33" s="2"/>
     </row>
-    <row r="34" spans="1:11">
+    <row r="34" spans="1:11" ht="32" thickTop="1" thickBot="1">
       <c r="A34" s="2"/>
-      <c r="B34" s="2"/>
-      <c r="C34" s="1"/>
-      <c r="E34" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="G34" s="2"/>
+      <c r="B34" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C34" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D34" s="10"/>
+      <c r="E34" s="10"/>
+      <c r="F34" s="10"/>
+      <c r="G34" s="2">
+        <v>6</v>
+      </c>
       <c r="H34" s="2"/>
       <c r="I34" s="2"/>
       <c r="J34" s="2"/>
       <c r="K34" s="2"/>
     </row>
-    <row r="35" spans="1:11">
+    <row r="35" spans="1:11" ht="16" thickTop="1">
       <c r="A35" s="2"/>
       <c r="B35" s="2"/>
       <c r="C35" s="1"/>
-      <c r="F35" t="s">
-        <v>50</v>
+      <c r="D35" t="s">
+        <v>52</v>
       </c>
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
@@ -1477,12 +1701,12 @@
       <c r="J35" s="2"/>
       <c r="K35" s="2"/>
     </row>
-    <row r="36" spans="1:11" ht="16" thickBot="1">
+    <row r="36" spans="1:11">
       <c r="A36" s="2"/>
       <c r="B36" s="2"/>
       <c r="C36" s="1"/>
-      <c r="F36" t="s">
-        <v>41</v>
+      <c r="E36" s="11" t="s">
+        <v>51</v>
       </c>
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
@@ -1490,29 +1714,25 @@
       <c r="J36" s="2"/>
       <c r="K36" s="2"/>
     </row>
-    <row r="37" spans="1:11" ht="32" thickTop="1" thickBot="1">
+    <row r="37" spans="1:11">
       <c r="A37" s="2"/>
-      <c r="B37" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="C37" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="D37" s="10"/>
-      <c r="E37" s="10"/>
-      <c r="F37" s="10"/>
+      <c r="B37" s="2"/>
+      <c r="C37" s="1"/>
+      <c r="F37" t="s">
+        <v>50</v>
+      </c>
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
       <c r="I37" s="2"/>
       <c r="J37" s="2"/>
       <c r="K37" s="2"/>
     </row>
-    <row r="38" spans="1:11" ht="16" thickTop="1">
+    <row r="38" spans="1:11" ht="16" thickBot="1">
       <c r="A38" s="2"/>
       <c r="B38" s="2"/>
       <c r="C38" s="1"/>
-      <c r="E38" t="s">
-        <v>54</v>
+      <c r="F38" t="s">
+        <v>41</v>
       </c>
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
@@ -1520,25 +1740,31 @@
       <c r="J38" s="2"/>
       <c r="K38" s="2"/>
     </row>
-    <row r="39" spans="1:11">
+    <row r="39" spans="1:11" ht="32" thickTop="1" thickBot="1">
       <c r="A39" s="2"/>
-      <c r="B39" s="2"/>
-      <c r="C39" s="1"/>
-      <c r="F39" t="s">
-        <v>53</v>
-      </c>
-      <c r="G39" s="2"/>
+      <c r="B39" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C39" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D39" s="10"/>
+      <c r="E39" s="10"/>
+      <c r="F39" s="10"/>
+      <c r="G39" s="2">
+        <v>1</v>
+      </c>
       <c r="H39" s="2"/>
       <c r="I39" s="2"/>
       <c r="J39" s="2"/>
       <c r="K39" s="2"/>
     </row>
-    <row r="40" spans="1:11">
+    <row r="40" spans="1:11" ht="16" thickTop="1">
       <c r="A40" s="2"/>
       <c r="B40" s="2"/>
       <c r="C40" s="1"/>
-      <c r="F40" t="s">
-        <v>42</v>
+      <c r="E40" t="s">
+        <v>54</v>
       </c>
       <c r="G40" s="2"/>
       <c r="H40" s="2"/>
@@ -1551,7 +1777,7 @@
       <c r="B41" s="2"/>
       <c r="C41" s="1"/>
       <c r="F41" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="G41" s="2"/>
       <c r="H41" s="2"/>
@@ -1562,10 +1788,10 @@
     <row r="42" spans="1:11">
       <c r="A42" s="2"/>
       <c r="B42" s="2"/>
-      <c r="C42" s="2"/>
-      <c r="D42" s="2"/>
-      <c r="E42" s="2"/>
-      <c r="F42" s="2"/>
+      <c r="C42" s="1"/>
+      <c r="F42" t="s">
+        <v>42</v>
+      </c>
       <c r="G42" s="2"/>
       <c r="H42" s="2"/>
       <c r="I42" s="2"/>
@@ -1575,10 +1801,10 @@
     <row r="43" spans="1:11">
       <c r="A43" s="2"/>
       <c r="B43" s="2"/>
-      <c r="C43" s="2"/>
-      <c r="D43" s="2"/>
-      <c r="E43" s="2"/>
-      <c r="F43" s="2"/>
+      <c r="C43" s="1"/>
+      <c r="F43" t="s">
+        <v>43</v>
+      </c>
       <c r="G43" s="2"/>
       <c r="H43" s="2"/>
       <c r="I43" s="2"/>
@@ -1586,9 +1812,7 @@
       <c r="K43" s="2"/>
     </row>
     <row r="44" spans="1:11">
-      <c r="A44" s="7" t="s">
-        <v>55</v>
-      </c>
+      <c r="A44" s="2"/>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
       <c r="D44" s="2"/>
@@ -1600,95 +1824,97 @@
       <c r="J44" s="2"/>
       <c r="K44" s="2"/>
     </row>
-    <row r="45" spans="1:11" ht="16" thickBot="1">
+    <row r="45" spans="1:11">
       <c r="A45" s="2"/>
-      <c r="B45" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C45" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="D45" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="E45" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="F45" s="7" t="s">
-        <v>39</v>
-      </c>
+      <c r="B45" s="2"/>
+      <c r="C45" s="2"/>
+      <c r="D45" s="2"/>
+      <c r="E45" s="2"/>
+      <c r="F45" s="2"/>
       <c r="G45" s="2"/>
       <c r="H45" s="2"/>
       <c r="I45" s="2"/>
       <c r="J45" s="2"/>
       <c r="K45" s="2"/>
     </row>
-    <row r="46" spans="1:11" ht="17" thickTop="1" thickBot="1">
-      <c r="A46" s="2"/>
-      <c r="B46" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="C46" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="D46" s="10"/>
-      <c r="E46" s="10"/>
-      <c r="F46" s="10"/>
+    <row r="46" spans="1:11">
+      <c r="A46" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B46" s="2"/>
+      <c r="C46" s="2"/>
+      <c r="D46" s="2"/>
+      <c r="E46" s="2"/>
+      <c r="F46" s="2"/>
       <c r="G46" s="2"/>
       <c r="H46" s="2"/>
       <c r="I46" s="2"/>
       <c r="J46" s="2"/>
       <c r="K46" s="2"/>
     </row>
-    <row r="47" spans="1:11" ht="16" thickTop="1">
+    <row r="47" spans="1:11" ht="16" thickBot="1">
       <c r="A47" s="2"/>
-      <c r="B47" s="2"/>
-      <c r="C47" s="1"/>
-      <c r="D47" t="s">
-        <v>58</v>
-      </c>
-      <c r="G47" s="2"/>
+      <c r="B47" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C47" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D47" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E47" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="F47" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="G47" s="2" t="s">
+        <v>72</v>
+      </c>
       <c r="H47" s="2"/>
       <c r="I47" s="2"/>
       <c r="J47" s="2"/>
       <c r="K47" s="2"/>
     </row>
-    <row r="48" spans="1:11" ht="16" thickBot="1">
+    <row r="48" spans="1:11" ht="17" thickTop="1" thickBot="1">
       <c r="A48" s="2"/>
-      <c r="B48" s="2"/>
-      <c r="C48" s="1"/>
-      <c r="D48" t="s">
-        <v>57</v>
-      </c>
-      <c r="G48" s="2"/>
+      <c r="B48" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C48" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D48" s="10"/>
+      <c r="E48" s="10"/>
+      <c r="F48" s="10"/>
+      <c r="G48" s="2">
+        <v>5</v>
+      </c>
       <c r="H48" s="2"/>
       <c r="I48" s="2"/>
       <c r="J48" s="2"/>
       <c r="K48" s="2"/>
     </row>
-    <row r="49" spans="1:11" ht="32" thickTop="1" thickBot="1">
+    <row r="49" spans="1:11" ht="16" thickTop="1">
       <c r="A49" s="2"/>
-      <c r="B49" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="C49" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="D49" s="10"/>
-      <c r="E49" s="10"/>
-      <c r="F49" s="10"/>
+      <c r="B49" s="2"/>
+      <c r="C49" s="1"/>
+      <c r="E49" t="s">
+        <v>58</v>
+      </c>
       <c r="G49" s="2"/>
       <c r="H49" s="2"/>
       <c r="I49" s="2"/>
       <c r="J49" s="2"/>
       <c r="K49" s="2"/>
     </row>
-    <row r="50" spans="1:11" ht="17" thickTop="1" thickBot="1">
+    <row r="50" spans="1:11" ht="16" thickBot="1">
       <c r="A50" s="2"/>
       <c r="B50" s="2"/>
       <c r="C50" s="1"/>
-      <c r="D50" t="s">
-        <v>56</v>
+      <c r="E50" t="s">
+        <v>57</v>
       </c>
       <c r="G50" s="2"/>
       <c r="H50" s="2"/>
@@ -1699,26 +1925,28 @@
     <row r="51" spans="1:11" ht="32" thickTop="1" thickBot="1">
       <c r="A51" s="2"/>
       <c r="B51" s="8" t="s">
-        <v>22</v>
+        <v>71</v>
       </c>
       <c r="C51" s="9" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D51" s="10"/>
       <c r="E51" s="10"/>
       <c r="F51" s="10"/>
-      <c r="G51" s="2"/>
+      <c r="G51" s="2">
+        <v>2</v>
+      </c>
       <c r="H51" s="2"/>
       <c r="I51" s="2"/>
       <c r="J51" s="2"/>
       <c r="K51" s="2"/>
     </row>
-    <row r="52" spans="1:11" ht="16" thickTop="1">
+    <row r="52" spans="1:11" ht="17" thickTop="1" thickBot="1">
       <c r="A52" s="2"/>
       <c r="B52" s="2"/>
       <c r="C52" s="1"/>
-      <c r="E52" s="11" t="s">
-        <v>59</v>
+      <c r="F52" t="s">
+        <v>56</v>
       </c>
       <c r="G52" s="2"/>
       <c r="H52" s="2"/>
@@ -1726,109 +1954,196 @@
       <c r="J52" s="2"/>
       <c r="K52" s="2"/>
     </row>
-    <row r="53" spans="1:11" ht="16" thickBot="1">
+    <row r="53" spans="1:11" ht="32" thickTop="1" thickBot="1">
       <c r="A53" s="2"/>
-      <c r="B53" s="2"/>
-      <c r="C53" s="1"/>
-      <c r="E53" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="G53" s="2"/>
+      <c r="B53" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C53" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D53" s="10"/>
+      <c r="E53" s="10"/>
+      <c r="F53" s="10"/>
+      <c r="G53" s="2">
+        <v>3</v>
+      </c>
       <c r="H53" s="2"/>
       <c r="I53" s="2"/>
       <c r="J53" s="2"/>
       <c r="K53" s="2"/>
     </row>
-    <row r="54" spans="1:11" ht="32" thickTop="1" thickBot="1">
-      <c r="B54" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="C54" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D54" s="10"/>
-      <c r="E54" s="10"/>
-      <c r="F54" s="10"/>
-    </row>
-    <row r="55" spans="1:11" ht="16" thickTop="1">
+    <row r="54" spans="1:11" ht="16" thickTop="1">
+      <c r="A54" s="2"/>
+      <c r="B54" s="2"/>
+      <c r="C54" s="1"/>
+      <c r="E54" s="11"/>
+      <c r="F54" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="G54" s="2"/>
+      <c r="H54" s="2"/>
+      <c r="I54" s="2"/>
+      <c r="J54" s="2"/>
+      <c r="K54" s="2"/>
+    </row>
+    <row r="55" spans="1:11" ht="16" thickBot="1">
+      <c r="A55" s="2"/>
       <c r="B55" s="2"/>
       <c r="C55" s="1"/>
-      <c r="D55" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="56" spans="1:11">
-      <c r="B56" s="2"/>
-      <c r="C56" s="1"/>
-      <c r="D56" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="57" spans="1:11" ht="16" thickBot="1">
+      <c r="E55" s="11"/>
+      <c r="F55" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="G55" s="2"/>
+      <c r="H55" s="2"/>
+      <c r="I55" s="2"/>
+      <c r="J55" s="2"/>
+      <c r="K55" s="2"/>
+    </row>
+    <row r="56" spans="1:11" ht="32" thickTop="1" thickBot="1">
+      <c r="B56" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C56" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D56" s="10"/>
+      <c r="E56" s="10"/>
+      <c r="F56" s="10"/>
+      <c r="G56">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" ht="16" thickTop="1">
       <c r="B57" s="2"/>
       <c r="C57" s="1"/>
-      <c r="E57" s="11" t="s">
+      <c r="D57" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" ht="16" thickBot="1">
+      <c r="B58" s="2"/>
+      <c r="C58" s="1"/>
+      <c r="E58" s="11"/>
+      <c r="F58" s="11" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="58" spans="1:11" ht="32" thickTop="1" thickBot="1">
-      <c r="B58" s="8" t="s">
+    <row r="59" spans="1:11" ht="17" thickTop="1" thickBot="1">
+      <c r="B59" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="C59" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="D59" s="10"/>
+      <c r="E59" s="10"/>
+      <c r="F59" s="10"/>
+      <c r="G59">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" ht="17" thickTop="1" thickBot="1">
+      <c r="B60" s="14"/>
+      <c r="C60" s="15"/>
+      <c r="D60" s="16"/>
+      <c r="E60" s="16"/>
+      <c r="F60" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" ht="32" thickTop="1" thickBot="1">
+      <c r="B61" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C58" s="9" t="s">
+      <c r="C61" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="D58" s="10"/>
-      <c r="E58" s="10"/>
-      <c r="F58" s="10"/>
-    </row>
-    <row r="59" spans="1:11" ht="17" thickTop="1" thickBot="1">
-      <c r="B59" s="2"/>
-      <c r="C59" s="1"/>
-      <c r="E59" t="s">
+      <c r="D61" s="10"/>
+      <c r="E61" s="10"/>
+      <c r="F61" s="10"/>
+      <c r="G61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" ht="17" thickTop="1" thickBot="1">
+      <c r="B62" s="2"/>
+      <c r="C62" s="1"/>
+      <c r="E62" t="s">
         <v>63</v>
-      </c>
-    </row>
-    <row r="60" spans="1:11" ht="32" thickTop="1" thickBot="1">
-      <c r="B60" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="C60" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="D60" s="10"/>
-      <c r="E60" s="10"/>
-      <c r="F60" s="10"/>
-    </row>
-    <row r="61" spans="1:11" ht="16" thickTop="1">
-      <c r="D61" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="62" spans="1:11" ht="16" thickBot="1">
-      <c r="D62" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="63" spans="1:11" ht="32" thickTop="1" thickBot="1">
       <c r="B63" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C63" s="13" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="D63" s="10"/>
       <c r="E63" s="10"/>
       <c r="F63" s="10"/>
+      <c r="G63">
+        <v>1</v>
+      </c>
     </row>
     <row r="64" spans="1:11" ht="16" thickTop="1">
       <c r="D64" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="65" spans="2:7" ht="16" thickBot="1">
+      <c r="E65" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="66" spans="2:7" ht="32" thickTop="1" thickBot="1">
+      <c r="B66" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C66" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D66" s="10"/>
+      <c r="E66" s="10"/>
+      <c r="F66" s="10"/>
+      <c r="G66">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="2:7" ht="16" thickTop="1">
+      <c r="E67" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="65" spans="4:4">
-      <c r="D65" t="s">
+    <row r="68" spans="2:7" ht="16" thickBot="1">
+      <c r="D68" t="s">
         <v>67</v>
+      </c>
+    </row>
+    <row r="69" spans="2:7" ht="32" thickTop="1" thickBot="1">
+      <c r="B69" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="C69" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="D69" s="10"/>
+      <c r="E69" s="10"/>
+      <c r="F69" s="10"/>
+      <c r="G69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="2:7" ht="16" thickTop="1">
+      <c r="D70" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="71" spans="2:7">
+      <c r="D71" t="s">
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -1840,21 +2155,4 @@
     </ext>
   </extLst>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
 </file>
</xml_diff>